<commit_message>
Hashing Konzept und High Level Konzept hinzugefügt
</commit_message>
<xml_diff>
--- a/Files/Tabellen/Verschlüsselung-Evaluationsmatrix.xlsx
+++ b/Files/Tabellen/Verschlüsselung-Evaluationsmatrix.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Kriterium</t>
   </si>
@@ -63,6 +63,18 @@
   </si>
   <si>
     <t>Total gewichtet</t>
+  </si>
+  <si>
+    <t>Gewicht:</t>
+  </si>
+  <si>
+    <t>1 (unwichtig) - 5 (sehr wichtig)</t>
+  </si>
+  <si>
+    <t>Punkte:</t>
+  </si>
+  <si>
+    <t>1 (sehr schlecht) - 10 (sehr gut)</t>
   </si>
 </sst>
 </file>
@@ -119,7 +131,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -165,15 +177,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -184,8 +226,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -466,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,158 +530,181 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>3</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>10</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>10</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>30</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>5</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>10</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>50</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>5</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>7</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>8</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>35</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>10</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>10</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>40</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>4</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>10</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>10</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>40</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="6">
+      <c r="B7" s="10"/>
+      <c r="C7" s="5">
         <v>47</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>39</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11">
+      <c r="B8" s="11"/>
+      <c r="C8" s="9">
         <v>195</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>155</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>